<commit_message>
First Mission 80% + Dialogue Handler 70%
</commit_message>
<xml_diff>
--- a/Capitain___Blood/WorkingFiles/FindMission.xlsx
+++ b/Capitain___Blood/WorkingFiles/FindMission.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6016CD1F-4A18-49B6-9008-B8B6F6D19207}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4DEF7-DDC8-4862-B7E2-9ECDCFBD2A23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -817,7 +817,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,27 +1981,27 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A3,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <f>FINDOrigin!B3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C3,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D3,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E3,DATA!$B:$B,))</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F3,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G3,DATA!$B:$B,))</f>
@@ -2027,15 +2027,15 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A4,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <f>FINDOrigin!B4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C4,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D4,DATA!$B:$B,))</f>
@@ -2085,19 +2085,19 @@
       </c>
       <c r="D4">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D5,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E5,DATA!$B:$B,))</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F5,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G5,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H5,DATA!$B:$B,))</f>
@@ -2119,7 +2119,7 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A6,DATA!$F:$F,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <f>FINDOrigin!B6</f>
@@ -2127,23 +2127,23 @@
       </c>
       <c r="C5">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C6,DATA!$D:$D,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D6,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E6,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F6,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G6,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H6,DATA!$B:$B,))</f>
@@ -2165,31 +2165,31 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A7,DATA!$F:$F,))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <f>FINDOrigin!B7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C7,DATA!$D:$D,))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D7,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E7,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F7,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G7,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H6">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H7,DATA!$B:$B,))</f>
@@ -2211,27 +2211,27 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A8,DATA!$F:$F,))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <f>FINDOrigin!B8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C8,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="G7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G8,DATA!$B:$B,))</f>
@@ -2239,49 +2239,49 @@
       </c>
       <c r="H7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K8,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A9,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <f>FINDOrigin!B9</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C9,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D9,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E9,DATA!$B:$B,))</f>
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F9,DATA!$B:$B,))</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G9,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H9,DATA!$B:$B,))</f>
@@ -2303,43 +2303,43 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A10,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <f>FINDOrigin!B10</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C10,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D10,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E10,DATA!$B:$B,))</f>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F10,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="G9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G10,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H10,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I10,DATA!$B:$B,))</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J10,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K10,DATA!$B:$B,))</f>
@@ -2349,39 +2349,39 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A11,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <f>FINDOrigin!B11</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C11,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D11,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E11,DATA!$B:$B,))</f>
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="F10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F11,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G11,DATA!$B:$B,))</f>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H11,DATA!$B:$B,))</f>
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I11,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J11,DATA!$B:$B,))</f>
@@ -2395,53 +2395,53 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A12,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <f>FINDOrigin!B12</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C12,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D12,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E12,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F12,DATA!$B:$B,))</f>
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G12,DATA!$B:$B,))</f>
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H12,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I12,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J12,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K12,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A13,DATA!$F:$F,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B12">
         <f>FINDOrigin!B13</f>
@@ -2453,35 +2453,35 @@
       </c>
       <c r="D12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="F12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K13,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B13">
         <f>FINDOrigin!B14</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C14,DATA!$D:$D,))</f>
@@ -2499,31 +2499,31 @@
       </c>
       <c r="D13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D14,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E14,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F14,DATA!$B:$B,))</f>
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G14,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="H13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H14,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I14,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J14,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K13">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K14,DATA!$B:$B,))</f>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B14">
         <f>FINDOrigin!B15</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C15,DATA!$D:$D,))</f>
@@ -2545,27 +2545,27 @@
       </c>
       <c r="D14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D15,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E15,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F15,DATA!$B:$B,))</f>
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G15,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="H14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H15,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="I14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I15,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J15,DATA!$B:$B,))</f>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B15">
         <f>FINDOrigin!B16</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C16,DATA!$D:$D,))</f>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="D15">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D16,DATA!$B:$B,))</f>
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E16,DATA!$B:$B,))</f>
@@ -2599,11 +2599,11 @@
       </c>
       <c r="F15">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F16,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G15">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G16,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="H15">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H16,DATA!$B:$B,))</f>
@@ -2625,11 +2625,11 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A17,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <f>FINDOrigin!B17</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C17,DATA!$D:$D,))</f>
@@ -2637,35 +2637,35 @@
       </c>
       <c r="D16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D17,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E17,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F17,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G17,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H17,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I17,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J17,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K17,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2683,19 +2683,19 @@
       </c>
       <c r="D17">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D18,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E18,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F18,DATA!$B:$B,))</f>
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G18,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H18,DATA!$B:$B,))</f>
@@ -2717,7 +2717,7 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A19,DATA!$F:$F,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <f>FINDOrigin!B19</f>
@@ -2729,35 +2729,35 @@
       </c>
       <c r="D18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="G18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K19,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2775,19 +2775,19 @@
       </c>
       <c r="D19">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D20,DATA!$B:$B,))</f>
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E19">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E20,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F19">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F20,DATA!$B:$B,))</f>
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="G19">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G20,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="H19">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H20,DATA!$B:$B,))</f>
@@ -2809,7 +2809,7 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A21,DATA!$F:$F,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B20">
         <f>FINDOrigin!B21</f>
@@ -2821,35 +2821,35 @@
       </c>
       <c r="D20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="E20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="G20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="H20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="I20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="J20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="K20">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K21,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
       </c>
       <c r="F21">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F22,DATA!$B:$B,))</f>
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G21">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G22,DATA!$B:$B,))</f>
@@ -2901,7 +2901,7 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A23,DATA!$F:$F,))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <f>FINDOrigin!B23</f>
@@ -2947,7 +2947,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A24,DATA!$F:$F,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23">
         <f>FINDOrigin!B24</f>
@@ -2955,27 +2955,27 @@
       </c>
       <c r="C23">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C24,DATA!$D:$D,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D24,DATA!$B:$B,))</f>
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E24,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F24,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G24,DATA!$B:$B,))</f>
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="H23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H24,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I24,DATA!$B:$B,))</f>
@@ -2993,11 +2993,11 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A25,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <f>FINDOrigin!B25</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C25,DATA!$D:$D,))</f>
@@ -3005,11 +3005,11 @@
       </c>
       <c r="D24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D25,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E25,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F25,DATA!$B:$B,))</f>
@@ -3017,23 +3017,23 @@
       </c>
       <c r="G24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G25,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H25,DATA!$B:$B,))</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I25,DATA!$B:$B,))</f>
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J25,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K25,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
       </c>
       <c r="B25">
         <f>FINDOrigin!B26</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C26,DATA!$D:$D,))</f>
@@ -3051,19 +3051,19 @@
       </c>
       <c r="D25">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D26,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E26,DATA!$B:$B,))</f>
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F25">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F26,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="G25">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G26,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="H25">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H26,DATA!$B:$B,))</f>
@@ -3085,11 +3085,11 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A27,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <f>FINDOrigin!B27</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C27,DATA!$D:$D,))</f>
@@ -3097,65 +3097,65 @@
       </c>
       <c r="D26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D27,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E27,DATA!$B:$B,))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F27,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G27,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H27,DATA!$B:$B,))</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I27,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J27,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K27,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A28,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <f>FINDOrigin!B28</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C28,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D28,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E27">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E28,DATA!$B:$B,))</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F28,DATA!$B:$B,))</f>
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="G27">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G28,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H28,DATA!$B:$B,))</f>
@@ -3177,27 +3177,27 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A29,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B28">
         <f>FINDOrigin!B29</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C28">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C29,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D29,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E29,DATA!$B:$B,))</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F29,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G29,DATA!$B:$B,))</f>
@@ -3223,31 +3223,31 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A30,DATA!$F:$F,))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B29">
         <f>FINDOrigin!B30</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C30,DATA!$D:$D,))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D30,DATA!$B:$B,))</f>
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E29">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E30,DATA!$B:$B,))</f>
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F29">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F30,DATA!$B:$B,))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G30,DATA!$B:$B,))</f>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H30,DATA!$B:$B,))</f>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="B30">
         <f>FINDOrigin!B31</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C31,DATA!$D:$D,))</f>
@@ -3285,19 +3285,19 @@
       </c>
       <c r="E30">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E31,DATA!$B:$B,))</f>
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="F30">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F31,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="G30">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G31,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H30">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H31,DATA!$B:$B,))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I30">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I31,DATA!$B:$B,))</f>
@@ -3315,11 +3315,11 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A32,DATA!$F:$F,))</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B31">
         <f>FINDOrigin!B32</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C32,DATA!$D:$D,))</f>
@@ -3327,34 +3327,494 @@
       </c>
       <c r="D31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="G31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="H31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J32,DATA!$B:$B,))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K32,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A33,DATA!$F:$F,))</f>
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <f>FINDOrigin!B33</f>
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C33,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D33,DATA!$B:$B,))</f>
+        <v>44</v>
+      </c>
+      <c r="E32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E33,DATA!$B:$B,))</f>
+        <v>109</v>
+      </c>
+      <c r="F32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F33,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G33,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H33,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I33,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J33,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K33,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A34,DATA!$F:$F,))</f>
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <f>FINDOrigin!B34</f>
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C34,DATA!$D:$D,))</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K34,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A35,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <f>FINDOrigin!B35</f>
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C35,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D35,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E35,DATA!$B:$B,))</f>
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F35,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G35,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="H34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H35,DATA!$B:$B,))</f>
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I35,DATA!$B:$B,))</f>
+        <v>98</v>
+      </c>
+      <c r="J34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J35,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K35,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A36,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <f>FINDOrigin!B36</f>
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C36,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D36,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E36,DATA!$B:$B,))</f>
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F36,DATA!$B:$B,))</f>
+        <v>44</v>
+      </c>
+      <c r="G35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G36,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H36,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I36,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J36,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K36,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A37,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <f>FINDOrigin!B37</f>
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C37,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D37,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E37,DATA!$B:$B,))</f>
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F37,DATA!$B:$B,))</f>
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G37,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H37,DATA!$B:$B,))</f>
+        <v>12</v>
+      </c>
+      <c r="I36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I37,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J37,DATA!$B:$B,))</f>
+        <v>44</v>
+      </c>
+      <c r="K36">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K37,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A38,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <f>FINDOrigin!B38</f>
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C38,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D38,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E38,DATA!$B:$B,))</f>
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F38,DATA!$B:$B,))</f>
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G38,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H38,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I38,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J38,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K38,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A39,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <f>FINDOrigin!B39</f>
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C39,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D39,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E39,DATA!$B:$B,))</f>
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F39,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G39,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H39,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I39,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J39,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K39,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A40,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <f>FINDOrigin!B40</f>
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C40,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D40,DATA!$B:$B,))</f>
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E40,DATA!$B:$B,))</f>
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F40,DATA!$B:$B,))</f>
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G40,DATA!$B:$B,))</f>
+        <v>44</v>
+      </c>
+      <c r="H39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H40,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I40,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J40,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K40,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A41,DATA!$F:$F,))</f>
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <f>FINDOrigin!B41</f>
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C41,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D41,DATA!$B:$B,))</f>
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E41,DATA!$B:$B,))</f>
+        <v>109</v>
+      </c>
+      <c r="F40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K41,DATA!$B:$B,))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>INDEX(DATA!$E:$E, MATCH(FINDOrigin!A42,DATA!$F:$F,))</f>
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <f>FINDOrigin!B42</f>
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <f>INDEX(DATA!$C:$C, MATCH(FINDOrigin!C42,DATA!$D:$D,))</f>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!D42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!E42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!F42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!G42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!H42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!I42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!J42,DATA!$B:$B,))</f>
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f>INDEX(DATA!$A:$A, MATCH(FINDOrigin!K42,DATA!$B:$B,))</f>
         <v>1</v>
       </c>
     </row>
@@ -3365,10 +3825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A32E93-B691-4469-B541-5AA78010B494}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3437,27 +3897,27 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -3477,218 +3937,182 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>133</v>
-      </c>
       <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3696,16 +4120,28 @@
         <v>127</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3713,16 +4149,25 @@
         <v>127</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="F15" t="s">
-        <v>58</v>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3730,51 +4175,51 @@
         <v>127</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3785,49 +4230,30 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>128</v>
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3838,49 +4264,48 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
         <v>61</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>44</v>
-      </c>
-      <c r="F20" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="I21" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="J21" t="s">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="K21" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3897,8 +4322,8 @@
         <v>44</v>
       </c>
       <c r="F22" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <f>"1"</f>
+        <v>1</v>
       </c>
       <c r="G22" t="s">
         <v>128</v>
@@ -3938,57 +4363,55 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
-        <v>133</v>
-      </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
         <v>128</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3996,102 +4419,106 @@
         <v>127</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" t="s">
         <v>44</v>
+      </c>
+      <c r="F26" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -4099,44 +4526,271 @@
         <v>127</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
         <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" t="s">
+        <v>98</v>
+      </c>
+      <c r="J35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>132</v>
       </c>
-      <c r="B32">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>1</v>
-      </c>
-      <c r="J32" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="B42">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1</v>
+      </c>
+      <c r="K42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4150,19 +4804,19 @@
           <x14:formula1>
             <xm:f>DATA!$B$4:$B$123</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:K582</xm:sqref>
+          <xm:sqref>D77:K582 D2:K42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49DEB12D-8CAC-4557-9E3B-E623FEA088A2}">
+          <x14:formula1>
+            <xm:f>DATA!$D$4:$D$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C77:C1048576 C2:C42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78BC8B1E-30E9-4D6A-B95A-C4062500DE24}">
           <x14:formula1>
             <xm:f>DATA!$F$3:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A582</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49DEB12D-8CAC-4557-9E3B-E623FEA088A2}">
-          <x14:formula1>
-            <xm:f>DATA!$D$4:$D$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>A77:A582 A2:A42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Random Speech Recognition 95%
</commit_message>
<xml_diff>
--- a/Capitain___Blood/WorkingFiles/FindMission.xlsx
+++ b/Capitain___Blood/WorkingFiles/FindMission.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2FB8CC-5305-4CCE-8BF6-32F56CB1F709}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616F04B6-6D74-4038-9047-69F03AE8F441}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3795" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="2" r:id="rId1"/>
@@ -3827,7 +3827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A32E93-B691-4469-B541-5AA78010B494}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>

</xml_diff>